<commit_message>
check for blank values
</commit_message>
<xml_diff>
--- a/custom/icds/location_rationalization/tests/data/Location Rationalisation Bad.xlsx
+++ b/custom/icds/location_rationalization/tests/data/Location Rationalisation Bad.xlsx
@@ -135,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -196,6 +196,19 @@
       <left style="thin">
         <color indexed="9"/>
       </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -229,7 +242,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -323,22 +336,25 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1428,7 +1444,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2353,56 +2369,106 @@
       <c r="Z18" s="29"/>
     </row>
     <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" s="31">
-        <v>1</v>
-      </c>
-      <c r="B19" s="32">
-        <v>1</v>
-      </c>
-      <c r="C19" s="32">
+      <c r="A19" s="26">
+        <v>1</v>
+      </c>
+      <c r="B19" s="27">
+        <v>1</v>
+      </c>
+      <c r="C19" s="27">
         <v>12</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="27">
         <v>12</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="27">
         <v>122</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="27">
         <v>122</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="9">
         <v>1221</v>
       </c>
-      <c r="H19" s="33">
+      <c r="H19" s="9">
         <v>1212</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="9">
         <v>12211</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="9">
         <v>12121</v>
       </c>
-      <c r="K19" t="s" s="34">
+      <c r="K19" t="s" s="10">
         <v>14</v>
       </c>
-      <c r="L19" t="s" s="34">
+      <c r="L19" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
-      <c r="Y19" s="35"/>
-      <c r="Z19" s="36"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="29"/>
+    </row>
+    <row r="20" ht="13.65" customHeight="1">
+      <c r="A20" s="31">
+        <v>1</v>
+      </c>
+      <c r="B20" s="31">
+        <v>1</v>
+      </c>
+      <c r="C20" s="31">
+        <v>12</v>
+      </c>
+      <c r="D20" s="31">
+        <v>12</v>
+      </c>
+      <c r="E20" s="31">
+        <v>122</v>
+      </c>
+      <c r="F20" s="31">
+        <v>122</v>
+      </c>
+      <c r="G20" s="32">
+        <v>1221</v>
+      </c>
+      <c r="H20" s="33">
+        <v>1221</v>
+      </c>
+      <c r="I20" s="33">
+        <v>12212</v>
+      </c>
+      <c r="J20" s="34"/>
+      <c r="K20" t="s" s="35">
+        <v>14</v>
+      </c>
+      <c r="L20" t="s" s="36">
+        <v>13</v>
+      </c>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="37"/>
+      <c r="W20" s="37"/>
+      <c r="X20" s="37"/>
+      <c r="Y20" s="37"/>
+      <c r="Z20" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>